<commit_message>
Final Update from Cisco
</commit_message>
<xml_diff>
--- a/AllenIdicula.xlsx
+++ b/AllenIdicula.xlsx
@@ -96,7 +96,7 @@
     <t>Reviewed concepts of Vmware, vCenter, QEMU, KVM, Abstract Hardware, the ability fo manage processes across servers, remote management, Open Stack, hypervisors, the difference between Network Attached Sotrage and Storage Area Networks.</t>
   </si>
   <si>
-    <t>q</t>
+    <t>Returned all materials…</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +537,7 @@
       </c>
       <c r="G2" s="8">
         <f>SUM(D2:D50)</f>
-        <v>1.380555555555556</v>
+        <v>1.4847222222222225</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -868,24 +868,31 @@
       <c r="A21" s="7">
         <v>0.625</v>
       </c>
-      <c r="B21" s="7"/>
+      <c r="B21" s="7">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="C21" s="4">
         <v>42093</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>-0.625</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="7">
+        <v>0.625</v>
+      </c>
       <c r="B22" s="7"/>
+      <c r="C22" s="4">
+        <v>42095</v>
+      </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.625</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>26</v>

</xml_diff>